<commit_message>
SO Invoice page actions TC in progress in LUI
</commit_message>
<xml_diff>
--- a/templates/DEVQAFF_LUI/SalesOrder_LUI.xlsx
+++ b/templates/DEVQAFF_LUI/SalesOrder_LUI.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_Automation\rsqasampleproj\templates\DEVQAFF_LUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4035D9-6AC4-4235-8260-02E2AAA983A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B0B1BC-5343-4342-A2BE-E802725B7E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="585" windowWidth="20430" windowHeight="7875" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25770" yWindow="5940" windowWidth="20430" windowHeight="7875" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
     <sheet name="AddLine" sheetId="2" r:id="rId2"/>
-    <sheet name="Invoice" sheetId="3" r:id="rId3"/>
-    <sheet name="AddHeader_SOAPI" sheetId="4" r:id="rId4"/>
-    <sheet name="AddLine_SOAPI" sheetId="5" r:id="rId5"/>
-    <sheet name="FirmAllLines" sheetId="6" r:id="rId6"/>
-    <sheet name="Allocate" sheetId="7" r:id="rId7"/>
-    <sheet name="PickPackShip" sheetId="8" r:id="rId8"/>
-    <sheet name="CreateInvoice" sheetId="9" r:id="rId9"/>
-    <sheet name="SelectApp" sheetId="10" r:id="rId10"/>
+    <sheet name="AddHeader_SOAPI" sheetId="4" r:id="rId3"/>
+    <sheet name="AddLine_SOAPI" sheetId="5" r:id="rId4"/>
+    <sheet name="FirmAllLines" sheetId="6" r:id="rId5"/>
+    <sheet name="Allocate" sheetId="7" r:id="rId6"/>
+    <sheet name="PickPackShip" sheetId="8" r:id="rId7"/>
+    <sheet name="CreateInvoice" sheetId="9" r:id="rId8"/>
+    <sheet name="SelectApp" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
   <si>
     <t>Customer</t>
   </si>
   <si>
-    <t>DJ-CUST1 (DJ-CUST1)</t>
-  </si>
-  <si>
     <t>ProductType</t>
   </si>
   <si>
@@ -51,18 +47,12 @@
     <t>Stock</t>
   </si>
   <si>
-    <t>DJ_Prod01_No-Track (No Track_MFG)</t>
-  </si>
-  <si>
     <t>Configured</t>
   </si>
   <si>
     <t>DivisionNumber</t>
   </si>
   <si>
-    <t>Conf_prod-No_track (purType)</t>
-  </si>
-  <si>
     <t>ProductTypeIndex</t>
   </si>
   <si>
@@ -120,21 +110,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>a5w0W000001M3f2QAC</t>
-  </si>
-  <si>
-    <t>a4i6T0000011FOvQAM</t>
-  </si>
-  <si>
-    <t>a6Q0W000001Q8bGUAS</t>
-  </si>
-  <si>
-    <t>a5N6T0000011RYnUAM</t>
-  </si>
-  <si>
-    <t>a5N6T0000011RZHUA2</t>
-  </si>
-  <si>
     <t>Transaction Type</t>
   </si>
   <si>
@@ -160,6 +135,33 @@
   </si>
   <si>
     <t>Sales Order Processes</t>
+  </si>
+  <si>
+    <t>AC5501_CUSTOMER (AC5501_CUSTOMER)</t>
+  </si>
+  <si>
+    <t>D1-AC</t>
+  </si>
+  <si>
+    <t>Automation5501-1 (Stock-Mfg-LotYesSerialYes)</t>
+  </si>
+  <si>
+    <t>Automation5501-2 (Mfg-LotYes)</t>
+  </si>
+  <si>
+    <t>a5w0W0000019TVB</t>
+  </si>
+  <si>
+    <t>a4i0W000001HpNn</t>
+  </si>
+  <si>
+    <t>a6Q0W000001Q8bG</t>
+  </si>
+  <si>
+    <t>a5N6T0000012ymD</t>
+  </si>
+  <si>
+    <t>a5N6T0000012ymN</t>
   </si>
 </sst>
 </file>
@@ -214,11 +216,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,7 +512,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -515,44 +520,20 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>901</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43534EE-E85B-4E5C-A117-543E5E92BCDD}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -572,13 +553,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -586,10 +567,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -597,10 +578,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -610,38 +591,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41AC6277-F927-4837-84C0-1EA27C4A85F9}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD32CE1-38EC-44D0-9A4E-C47D6C3C0999}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -658,51 +611,51 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H2" t="b">
         <v>1</v>
@@ -713,12 +666,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FE198D-50FF-4D5C-9501-D9360F83F0E1}">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,72 +693,72 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -823,33 +776,33 @@
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="H3" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="I3">
         <v>2</v>
@@ -872,7 +825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{329BA206-545B-4BD9-86D8-6F87FF991516}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -888,16 +841,16 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
@@ -908,7 +861,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3628B4E-034C-442C-A3BB-0A2CD2EC1698}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -925,18 +878,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
@@ -950,7 +903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99FA1BCC-1BF3-42D7-9336-2B7B0E5FE772}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -965,18 +918,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -990,7 +943,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F823134-5A38-4425-8DE7-842F0EC42E7F}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1005,21 +958,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -1028,7 +981,32 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43534EE-E85B-4E5C-A117-543E5E92BCDD}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>